<commit_message>
checks fields, adds some min and max values
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_redd_metadata.xlsx
+++ b/data-raw/metadata/feather_redd_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-redd\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0766DE6A-50D6-4E5D-9B09-AF5FA33FE7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F900BC5-1AE6-4EC2-B9F5-60B508812957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="65">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -139,9 +139,6 @@
     <t>numebr of fish on redd</t>
   </si>
   <si>
-    <t>number of redds</t>
-  </si>
-  <si>
     <t>redds</t>
   </si>
   <si>
@@ -212,6 +209,18 @@
   </si>
   <si>
     <t>interval</t>
+  </si>
+  <si>
+    <t>feather_redd</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>number of redds observed</t>
+  </si>
+  <si>
+    <t>salmon</t>
   </si>
 </sst>
 </file>
@@ -666,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -682,7 +691,8 @@
     <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
     <col min="10" max="10" width="16" style="5" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="1021" width="19.6640625" style="1"/>
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
@@ -733,24 +743,43 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="6"/>
+      <c r="L2" s="6">
+        <v>41891</v>
+      </c>
+      <c r="M2" s="6">
+        <v>45259</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -758,13 +787,16 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -775,13 +807,16 @@
         <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
@@ -792,36 +827,48 @@
         <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="H7" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -829,10 +876,28 @@
         <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -840,22 +905,31 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -863,22 +937,25 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
@@ -886,22 +963,25 @@
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -909,22 +989,25 @@
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -932,22 +1015,25 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -955,22 +1041,25 @@
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -978,22 +1067,25 @@
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -1001,22 +1093,25 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="31" x14ac:dyDescent="0.35">
@@ -1024,22 +1119,25 @@
         <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="31" x14ac:dyDescent="0.35">
@@ -1047,22 +1145,25 @@
         <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1070,10 +1171,13 @@
         <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="31" x14ac:dyDescent="0.35">
@@ -1081,10 +1185,13 @@
         <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continues cleaning make metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_redd_metadata.xlsx
+++ b/data-raw/metadata/feather_redd_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-redd\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F900BC5-1AE6-4EC2-B9F5-60B508812957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1242CDCA-5198-4E39-8D66-8D518C679E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -88,12 +88,6 @@
     <t>file_number</t>
   </si>
   <si>
-    <t>number_of_redds</t>
-  </si>
-  <si>
-    <t>number_of_salmon</t>
-  </si>
-  <si>
     <t>depth_m</t>
   </si>
   <si>
@@ -221,6 +215,15 @@
   </si>
   <si>
     <t>salmon</t>
+  </si>
+  <si>
+    <t>number_redds</t>
+  </si>
+  <si>
+    <t>number_salmon</t>
+  </si>
+  <si>
+    <t>decimal degrees</t>
   </si>
 </sst>
 </file>
@@ -675,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -743,19 +746,19 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="6">
@@ -770,16 +773,16 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -787,16 +790,16 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -804,19 +807,19 @@
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
@@ -824,74 +827,74 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L7" s="5">
         <v>0</v>
       </c>
       <c r="M7" s="5">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L8" s="5">
         <v>0</v>
@@ -902,28 +905,28 @@
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L9" s="5">
         <v>0</v>
@@ -934,264 +937,342 @@
     </row>
     <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
         <v>50</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="L11" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M11" s="5">
+        <v>2.74</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="D19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-writes csv and metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_redd_metadata.xlsx
+++ b/data-raw/metadata/feather_redd_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-redd\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51010C94-4686-4C63-9C1E-77F7BF589A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD4A56C-D23A-4040-8E58-E6B09739C599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="19200" windowHeight="11170" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4490" yWindow="1360" windowWidth="19200" windowHeight="11170" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMF19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="15" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>38</v>
@@ -1188,18 +1188,18 @@
         <v>37</v>
       </c>
       <c r="L15" s="5">
+        <v>-127.48869999999999</v>
+      </c>
+      <c r="M15" s="5">
         <v>0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>39.695790000000002</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
@@ -1220,10 +1220,10 @@
         <v>37</v>
       </c>
       <c r="L16" s="5">
-        <v>-127.48869999999999</v>
+        <v>0</v>
       </c>
       <c r="M16" s="5">
-        <v>0</v>
+        <v>39.695790000000002</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="31" x14ac:dyDescent="0.35">
@@ -1309,19 +1309,19 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1016" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:C1016 C1:C16" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1016" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:E1016 E1:E16" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1016" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F1016 F1:F16" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H17:H1048576 H1:H16" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates metadata and adds location and survey week
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_redd_metadata.xlsx
+++ b/data-raw/metadata/feather_redd_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-redd\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD4A56C-D23A-4040-8E58-E6B09739C599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E958D0A4-B3C0-4AF2-B585-1D5B5BEA4044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4490" yWindow="1360" windowWidth="19200" windowHeight="11170" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="74">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -233,6 +233,21 @@
   </si>
   <si>
     <t>feet</t>
+  </si>
+  <si>
+    <t>survey_wk</t>
+  </si>
+  <si>
+    <t>Week of survey</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Name of survey location site</t>
   </si>
 </sst>
 </file>
@@ -685,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMF19"/>
+  <dimension ref="A1:AMF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -780,74 +795,52 @@
     </row>
     <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5">
-        <v>15</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>31</v>
@@ -862,7 +855,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>33</v>
@@ -871,15 +864,15 @@
         <v>0</v>
       </c>
       <c r="M5" s="5">
-        <v>1.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>31</v>
@@ -893,8 +886,8 @@
       <c r="F6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>34</v>
+      <c r="G6" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>33</v>
@@ -906,12 +899,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>31</v>
@@ -926,24 +919,24 @@
         <v>31</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L7" s="5">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="M7" s="5">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>31</v>
@@ -957,25 +950,25 @@
       <c r="F8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>36</v>
+      <c r="G8" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L8" s="5">
         <v>0</v>
       </c>
       <c r="M8" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
@@ -990,24 +983,24 @@
         <v>31</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L9" s="5">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="M9" s="5">
-        <v>90</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>
@@ -1031,15 +1024,15 @@
         <v>0</v>
       </c>
       <c r="M10" s="5">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
@@ -1068,10 +1061,10 @@
     </row>
     <row r="12" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1095,15 +1088,15 @@
         <v>0</v>
       </c>
       <c r="M12" s="5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>31</v>
@@ -1118,24 +1111,24 @@
         <v>31</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L13" s="5">
         <v>0</v>
       </c>
       <c r="M13" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -1150,27 +1143,27 @@
         <v>31</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L14" s="5">
         <v>0</v>
       </c>
       <c r="M14" s="5">
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>66</v>
@@ -1179,30 +1172,30 @@
         <v>32</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L15" s="5">
-        <v>-127.48869999999999</v>
+        <v>0</v>
       </c>
       <c r="M15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>66</v>
@@ -1211,117 +1204,181 @@
         <v>32</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L16" s="5">
         <v>0</v>
       </c>
       <c r="M16" s="5">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="5">
+        <v>-127.48869999999999</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
         <v>39.695790000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L19" s="5">
         <v>49.82</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M19" s="5">
         <v>134.77000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="31" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L20" s="5">
         <v>0.41</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M20" s="5">
         <v>9.84</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="D21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:C1016 C1:C16" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1018" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:E1016 E1:E16" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1018" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F1016 F1:F16" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1018" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H17:H1048576 H1:H16" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>